<commit_message>
fix oubli "effort" dans rapport str
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/Report Str.xlsx
+++ b/lib/PHPExcel/templates/Report Str.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -331,55 +331,55 @@
     <t>Contrôle effort</t>
   </si>
   <si>
+    <t>Système M.T.S. hydraulique de capacité 250 kN.</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Préfixe Éprouvette</t>
+  </si>
+  <si>
+    <t>Nom Éprouvette</t>
+  </si>
+  <si>
+    <t>Eprouvettes usinées par Metcut Research Inc, sous référence : xxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>Str</t>
+  </si>
+  <si>
+    <t>Avant la spécif</t>
+  </si>
+  <si>
+    <t>Après spécif</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> et Instructions client.</t>
+  </si>
+  <si>
+    <t>Joachim GALIPAUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASTM E606-12, </t>
+  </si>
+  <si>
+    <t>Voir cellule $K et $L</t>
+  </si>
+  <si>
+    <t>Essais de fatigue sur xxxxx éprouvettes, matériau fourni par xxxxxxx.</t>
+  </si>
+  <si>
+    <t>Requête client</t>
+  </si>
+  <si>
     <t>Essai en déformation axiale imposée jusqu'à 85000 cycles et passage en contrôle</t>
   </si>
   <si>
-    <t>Système M.T.S. hydraulique de capacité 250 kN.</t>
-  </si>
-  <si>
-    <t>jusqu'à rupture.</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>ET</t>
-  </si>
-  <si>
-    <t>Préfixe Éprouvette</t>
-  </si>
-  <si>
-    <t>Nom Éprouvette</t>
-  </si>
-  <si>
-    <t>Eprouvettes usinées par Metcut Research Inc, sous référence : xxxxxxxxxx</t>
-  </si>
-  <si>
-    <t>Str</t>
-  </si>
-  <si>
-    <t>Avant la spécif</t>
-  </si>
-  <si>
-    <t>Après spécif</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> et Instructions client.</t>
-  </si>
-  <si>
-    <t>Joachim GALIPAUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASTM E606-12, </t>
-  </si>
-  <si>
-    <t>Voir cellule $K et $L</t>
-  </si>
-  <si>
-    <t>Essais de fatigue sur xxxxx éprouvettes, matériau fourni par xxxxxxx.</t>
-  </si>
-  <si>
-    <t>Requête client</t>
+    <t>effort jusqu'à rupture.</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1329,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1470,12 +1472,12 @@
         <v>17</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="29"/>
     </row>
@@ -1499,10 +1501,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K18" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1513,13 +1515,13 @@
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K19" s="80" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L19" s="80" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1598,12 +1600,12 @@
         <v>4</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E31" s="27" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1697,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
@@ -1739,7 +1741,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H51" s="29"/>
       <c r="I51" s="30"/>
@@ -1827,7 +1829,7 @@
     </row>
     <row r="5" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="23"/>
@@ -1835,7 +1837,7 @@
     </row>
     <row r="6" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="23"/>
@@ -1906,7 +1908,7 @@
     <row r="14" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
       <c r="B14" s="85" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="87"/>
@@ -1914,7 +1916,7 @@
     <row r="15" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="70"/>
       <c r="B15" s="86" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="88"/>
@@ -1929,7 +1931,7 @@
     </row>
     <row r="17" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" s="40" t="s">
@@ -1939,7 +1941,7 @@
     </row>
     <row r="18" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="40" t="s">
@@ -1949,7 +1951,7 @@
     </row>
     <row r="19" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="37"/>
       <c r="C19" s="40" t="s">
@@ -1969,7 +1971,7 @@
     </row>
     <row r="21" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" s="37"/>
       <c r="C21" s="40" t="s">
@@ -1979,7 +1981,7 @@
     </row>
     <row r="22" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" s="37"/>
       <c r="C22" s="41"/>
@@ -1987,7 +1989,7 @@
     </row>
     <row r="23" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" s="37"/>
       <c r="C23" s="40" t="s">
@@ -2416,7 +2418,7 @@
     <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="76"/>
       <c r="D1" s="76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>0</v>

</xml_diff>